<commit_message>
All Changes done for creative delivery sql nan to S3
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
     <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId2"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="70">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -1071,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,4 +1564,502 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes done for Creative Conversion
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
-    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId2"/>
-    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId3"/>
+    <sheet name="Creative_Conversion_S3_Mapper" sheetId="4" r:id="rId2"/>
+    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId3"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="70">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -591,7 +592,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E25"/>
+      <selection sqref="A1:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,6 +1070,487 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -1566,12 +2048,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Test Cases for Trait Conversion sql Nan to S3 and Datastream
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="748" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
     <sheet name="Creative_Conversion_S3_Mapper" sheetId="4" r:id="rId2"/>
-    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId3"/>
-    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId4"/>
+    <sheet name="Trait_Conversion_Mapper" sheetId="6" r:id="rId3"/>
+    <sheet name="Trait_Conversion_S3_Mapper" sheetId="7" r:id="rId4"/>
+    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId5"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="79">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -237,6 +239,33 @@
   </si>
   <si>
     <t>Total_Cost</t>
+  </si>
+  <si>
+    <t>Trait_ID</t>
+  </si>
+  <si>
+    <t>Trait_Name</t>
+  </si>
+  <si>
+    <t>Line Item Flight Start Date</t>
+  </si>
+  <si>
+    <t>Line Item Flight End Date</t>
+  </si>
+  <si>
+    <t>Line Item Status</t>
+  </si>
+  <si>
+    <t>Segment ID</t>
+  </si>
+  <si>
+    <t>Segment Name</t>
+  </si>
+  <si>
+    <t>Publisher Name</t>
+  </si>
+  <si>
+    <t>Currency</t>
   </si>
 </sst>
 </file>
@@ -592,7 +621,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E27"/>
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,6 +1580,831 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -2048,7 +2902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added changes for the Trait Delivery Sql Nan to S3 and Datastream
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="748" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <sheet name="Trait_Conversion_Mapper" sheetId="6" r:id="rId3"/>
     <sheet name="Trait_Conversion_S3_Mapper" sheetId="7" r:id="rId4"/>
     <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId5"/>
-    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId6"/>
+    <sheet name="Trait_Delivery_Mapper" sheetId="8" r:id="rId6"/>
+    <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId7"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="79">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -1995,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2904,6 +2906,866 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Code Changes for Domain Conversion sql nan to s3 and datastream
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Trait_Conversion_S3_Mapper" sheetId="7" r:id="rId4"/>
     <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId5"/>
     <sheet name="Trait_Delivery_Mapper" sheetId="8" r:id="rId6"/>
-    <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId7"/>
-    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId8"/>
+    <sheet name="Domain_Conversion_Mapper" sheetId="10" r:id="rId7"/>
+    <sheet name="Domain_Conversion_S3_Mapper" sheetId="11" r:id="rId8"/>
+    <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId9"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="81">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -268,6 +270,12 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Site_URL</t>
+  </si>
+  <si>
+    <t>Site Key</t>
   </si>
 </sst>
 </file>
@@ -623,7 +631,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+      <selection activeCell="A2" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,12 +1108,510 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E27"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,6 +2084,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2908,7 +3415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3335,6 +3842,1001 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -3762,502 +5264,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added code changes for Domain Delivery Sql nan to S3 and Data stream
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
     <sheet name="Creative_Conversion_S3_Mapper" sheetId="4" r:id="rId2"/>
-    <sheet name="Trait_Conversion_Mapper" sheetId="6" r:id="rId3"/>
-    <sheet name="Trait_Conversion_S3_Mapper" sheetId="7" r:id="rId4"/>
-    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId5"/>
-    <sheet name="Trait_Delivery_Mapper" sheetId="8" r:id="rId6"/>
-    <sheet name="Domain_Conversion_Mapper" sheetId="10" r:id="rId7"/>
-    <sheet name="Domain_Conversion_S3_Mapper" sheetId="11" r:id="rId8"/>
-    <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId9"/>
-    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId10"/>
+    <sheet name="Creative_Delivery_Mapper" sheetId="2" r:id="rId3"/>
+    <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId4"/>
+    <sheet name="Trait_Conversion_Mapper" sheetId="6" r:id="rId5"/>
+    <sheet name="Trait_Conversion_S3_Mapper" sheetId="7" r:id="rId6"/>
+    <sheet name="Trait_Delivery_Mapper" sheetId="8" r:id="rId7"/>
+    <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId8"/>
+    <sheet name="Domain_Conversion_Mapper" sheetId="10" r:id="rId9"/>
+    <sheet name="Domain_Conversion_S3_Mapper" sheetId="11" r:id="rId10"/>
+    <sheet name="Domain_Delivery_Mapper" sheetId="12" r:id="rId11"/>
+    <sheet name="Domain_Delivery_S3_Mapper" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="81">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -1113,7 +1115,505 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,6 +1644,521 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1552,10 +2567,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>0</v>
@@ -1564,15 +2579,15 @@
         <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>0</v>
@@ -1586,18 +2601,35 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2090,6 +3122,1003 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2500,7 +4529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2913,505 +4942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -3841,1002 +5372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -5264,4 +5800,501 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Company store stream and nan to s3 modifications for double quotes
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\datorama-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\DatoramaMain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2316" windowHeight="7092" tabRatio="885" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Domain_Conversion_S3_Mapper" sheetId="11" r:id="rId8"/>
     <sheet name="Trait_Delivery_S3_Mapper" sheetId="9" r:id="rId9"/>
     <sheet name="Creative_Delivery_S3_Mapper" sheetId="3" r:id="rId10"/>
+    <sheet name="Company_Store_Mapper" sheetId="12" r:id="rId11"/>
+    <sheet name="Company_Store_S3_Mapper" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="101">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -276,6 +278,66 @@
   </si>
   <si>
     <t>Site Key</t>
+  </si>
+  <si>
+    <t>Advertiser</t>
+  </si>
+  <si>
+    <t>BU_Name</t>
+  </si>
+  <si>
+    <t>Company ID</t>
+  </si>
+  <si>
+    <t>Company_ID</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Agency ID</t>
+  </si>
+  <si>
+    <t>Agency_ID</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>Agency_Name</t>
+  </si>
+  <si>
+    <t>Division ID</t>
+  </si>
+  <si>
+    <t>Division_ID</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Region ID</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Time Zone</t>
+  </si>
+  <si>
+    <t>Division_Name</t>
+  </si>
+  <si>
+    <t>Region_ID</t>
+  </si>
+  <si>
+    <t>Region_Name</t>
+  </si>
+  <si>
+    <t>TimeZone_Name</t>
+  </si>
+  <si>
+    <t>Company_Name</t>
   </si>
 </sst>
 </file>
@@ -634,16 +696,16 @@
       <selection activeCell="A2" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -677,7 +739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -694,7 +756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -711,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -728,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -745,7 +807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -762,7 +824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -779,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -796,7 +858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -813,7 +875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -830,7 +892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -847,7 +909,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -864,7 +926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -881,7 +943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -898,7 +960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -915,7 +977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -932,7 +994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -949,7 +1011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -966,7 +1028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -983,7 +1045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1000,7 +1062,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1017,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1034,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1051,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1068,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1085,7 +1147,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1116,16 +1178,16 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1204,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1176,7 +1238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1227,7 +1289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1244,7 +1306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1278,7 +1340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1295,7 +1357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1312,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1346,7 +1408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1363,7 +1425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1380,7 +1442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1397,7 +1459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1431,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1448,7 +1510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1465,7 +1527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1482,7 +1544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1516,7 +1578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1533,7 +1595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1550,7 +1612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
@@ -1567,7 +1629,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
@@ -1584,7 +1646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -1598,6 +1660,459 @@
         <v>66</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1614,16 +2129,16 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +2155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +2172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1674,7 +2189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1691,7 +2206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1708,7 +2223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1725,7 +2240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1742,7 +2257,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1759,7 +2274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1776,7 +2291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1793,7 +2308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1810,7 +2325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1827,7 +2342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1844,7 +2359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1861,7 +2376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -1878,7 +2393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1895,7 +2410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1912,7 +2427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1929,7 +2444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1946,7 +2461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1963,7 +2478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1980,7 +2495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1997,7 +2512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -2014,7 +2529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -2031,7 +2546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -2048,7 +2563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -2065,7 +2580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -2096,15 +2611,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2121,7 +2636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2138,7 +2653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -2155,7 +2670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -2172,7 +2687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -2189,7 +2704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -2206,7 +2721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -2223,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2240,7 +2755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -2257,7 +2772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -2274,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -2291,7 +2806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -2308,7 +2823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -2325,7 +2840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -2342,7 +2857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -2359,7 +2874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
@@ -2376,7 +2891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -2393,7 +2908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -2410,7 +2925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -2427,7 +2942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
@@ -2444,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>78</v>
       </c>
@@ -2461,7 +2976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -2478,7 +2993,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -2508,16 +3023,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2534,7 +3049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2551,7 +3066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2568,7 +3083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2585,7 +3100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2602,7 +3117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2619,7 +3134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2636,7 +3151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -2653,7 +3168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -2670,7 +3185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2687,7 +3202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2704,7 +3219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -2721,7 +3236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -2738,7 +3253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2755,7 +3270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2772,7 +3287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -2789,7 +3304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -2806,7 +3321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -2823,7 +3338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -2840,7 +3355,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -2857,7 +3372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -2874,7 +3389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2891,7 +3406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -2921,16 +3436,16 @@
       <selection sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +3462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2964,7 +3479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -2981,7 +3496,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -2998,7 +3513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -3015,7 +3530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -3032,7 +3547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -3049,7 +3564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3066,7 +3581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -3083,7 +3598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -3100,7 +3615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -3117,7 +3632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -3134,7 +3649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -3151,7 +3666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -3168,7 +3683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -3185,7 +3700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -3202,7 +3717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -3219,7 +3734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -3236,7 +3751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -3253,7 +3768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -3270,7 +3785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -3287,7 +3802,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -3304,7 +3819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -3321,7 +3836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -3338,7 +3853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -3355,7 +3870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -3372,7 +3887,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -3389,7 +3904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -3419,16 +3934,16 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3445,7 +3960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3462,7 +3977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -3479,7 +3994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -3496,7 +4011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -3513,7 +4028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -3530,7 +4045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -3547,7 +4062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3564,7 +4079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -3581,7 +4096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -3598,7 +4113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -3615,7 +4130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -3632,7 +4147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -3649,7 +4164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
@@ -3666,7 +4181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -3683,7 +4198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -3700,7 +4215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -3717,7 +4232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>76</v>
       </c>
@@ -3734,7 +4249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -3751,7 +4266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -3768,7 +4283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -3785,7 +4300,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
@@ -3802,7 +4317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -3819,7 +4334,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -3849,15 +4364,15 @@
       <selection sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3874,7 +4389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3891,7 +4406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
@@ -3908,7 +4423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -3925,7 +4440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -3942,7 +4457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -3959,7 +4474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>43</v>
       </c>
@@ -3976,7 +4491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3993,7 +4508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>45</v>
       </c>
@@ -4010,7 +4525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -4027,7 +4542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -4044,7 +4559,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -4061,7 +4576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -4078,7 +4593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -4095,7 +4610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -4112,7 +4627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
@@ -4129,7 +4644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -4146,7 +4661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
@@ -4163,7 +4678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -4180,7 +4695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -4197,7 +4712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -4214,7 +4729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
@@ -4231,7 +4746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -4248,7 +4763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -4265,7 +4780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -4282,7 +4797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>80</v>
       </c>
@@ -4299,7 +4814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -4316,7 +4831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -4342,20 +4857,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4372,7 +4887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4389,7 +4904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -4406,7 +4921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -4423,7 +4938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -4440,7 +4955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4457,7 +4972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -4474,7 +4989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -4491,7 +5006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -4508,7 +5023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4525,7 +5040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -4542,7 +5057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -4559,7 +5074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -4576,7 +5091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -4593,7 +5108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -4610,7 +5125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -4627,7 +5142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -4644,7 +5159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -4661,7 +5176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -4678,7 +5193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -4695,7 +5210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -4712,7 +5227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -4729,7 +5244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -4746,7 +5261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -4763,7 +5278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -4780,7 +5295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -4797,7 +5312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -4814,7 +5329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -4844,16 +5359,16 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4870,7 +5385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -4887,7 +5402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -4904,7 +5419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -4921,7 +5436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -4938,7 +5453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4955,7 +5470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -4972,7 +5487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -4989,7 +5504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -5006,7 +5521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -5023,7 +5538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -5040,7 +5555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -5057,7 +5572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -5074,7 +5589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -5091,7 +5606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -5108,7 +5623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -5125,7 +5640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -5142,7 +5657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -5159,7 +5674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -5176,7 +5691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -5193,7 +5708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -5210,7 +5725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -5227,7 +5742,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>64</v>
       </c>
@@ -5244,7 +5759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Added changes for domain delivery and domain conversion plus additional mapping changes
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="86">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -278,6 +278,21 @@
   </si>
   <si>
     <t>Site Key</t>
+  </si>
+  <si>
+    <t>Trait Impressions</t>
+  </si>
+  <si>
+    <t>Trait Clicks</t>
+  </si>
+  <si>
+    <t>Trait Cost</t>
+  </si>
+  <si>
+    <t>Trait Click Based Conversions</t>
+  </si>
+  <si>
+    <t>Trait View Based Conversions</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1575,7 @@
         <v>79</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -1612,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2058,7 +2073,7 @@
         <v>79</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -2127,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,7 +2588,7 @@
         <v>79</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -4122,7 +4137,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4492,7 +4507,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
@@ -4509,7 +4524,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>29</v>
@@ -4533,7 +4548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -4947,7 +4962,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5318,7 +5333,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -5335,7 +5350,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>64</v>
@@ -5352,7 +5367,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>65</v>
@@ -5806,8 +5821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6251,7 +6266,7 @@
         <v>79</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added code changes to make the framework branch work
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="111">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Site_URL</t>
   </si>
   <si>
-    <t>Site Key</t>
-  </si>
-  <si>
     <t>Trait Impressions</t>
   </si>
   <si>
@@ -355,6 +352,24 @@
   </si>
   <si>
     <t>Time Zone</t>
+  </si>
+  <si>
+    <t>Domain Click Based Conversions</t>
+  </si>
+  <si>
+    <t>Domain View Based Conversions</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Domain Impressions</t>
+  </si>
+  <si>
+    <t>Domain Clicks</t>
+  </si>
+  <si>
+    <t>Domain Cost</t>
   </si>
 </sst>
 </file>
@@ -1621,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2075,7 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>79</v>
@@ -2077,7 +2092,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
@@ -2094,7 +2109,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>29</v>
@@ -2616,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3056,7 +3071,7 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>79</v>
@@ -3073,7 +3088,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>63</v>
@@ -3090,7 +3105,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>64</v>
@@ -3107,7 +3122,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>65</v>
@@ -5496,7 +5511,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
@@ -5513,7 +5528,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>29</v>
@@ -5950,7 +5965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -5992,10 +6007,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -6009,10 +6024,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -6026,10 +6041,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -6043,10 +6058,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
@@ -6060,10 +6075,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -6077,10 +6092,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
@@ -6094,10 +6109,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>0</v>
@@ -6111,10 +6126,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
@@ -6128,10 +6143,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -6145,10 +6160,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -6211,10 +6226,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -6228,10 +6243,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -6245,10 +6260,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -6262,10 +6277,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
@@ -6279,10 +6294,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -6296,10 +6311,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
@@ -6313,10 +6328,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>0</v>
@@ -6330,10 +6345,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
@@ -6347,10 +6362,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -6364,10 +6379,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -6760,7 +6775,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -6777,7 +6792,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>64</v>
@@ -6794,7 +6809,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Modified the mapping of creative file
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="108">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -222,12 +222,6 @@
     <t>Currency (Original)</t>
   </si>
   <si>
-    <t>Total_Click Based Conversions</t>
-  </si>
-  <si>
-    <t>Total_View Based Conversions</t>
-  </si>
-  <si>
     <t>Impressions</t>
   </si>
   <si>
@@ -240,15 +234,6 @@
     <t>DOUBLE</t>
   </si>
   <si>
-    <t>Total_Impressions</t>
-  </si>
-  <si>
-    <t>Total_Clicks</t>
-  </si>
-  <si>
-    <t>Total_Cost</t>
-  </si>
-  <si>
     <t>Trait_ID</t>
   </si>
   <si>
@@ -370,6 +355,12 @@
   </si>
   <si>
     <t>Domain Cost</t>
+  </si>
+  <si>
+    <t>Click Based Conversions</t>
+  </si>
+  <si>
+    <t>View Based Conversions</t>
   </si>
 </sst>
 </file>
@@ -725,7 +716,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A27"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1155,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -1181,7 +1172,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
@@ -1493,10 +1484,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -1510,10 +1501,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>0</v>
@@ -1578,10 +1569,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -1595,10 +1586,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>0</v>
@@ -1612,16 +1603,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -1636,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +1862,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -1888,7 +1879,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
@@ -1905,7 +1896,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -2075,10 +2066,10 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -2092,7 +2083,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>27</v>
@@ -2109,7 +2100,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>29</v>
@@ -2573,10 +2564,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -3071,10 +3062,10 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -3088,10 +3079,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>0</v>
@@ -3105,10 +3096,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -3122,16 +3113,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>7</v>
@@ -3586,10 +3577,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>1</v>
@@ -3603,10 +3594,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>0</v>
@@ -3620,10 +3611,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -3637,16 +3628,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>7</v>
@@ -4143,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4583,10 +4574,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -4600,10 +4591,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -4617,16 +4608,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -5082,10 +5073,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>0</v>
@@ -5099,10 +5090,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>0</v>
@@ -5116,16 +5107,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
@@ -5375,7 +5366,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -5392,7 +5383,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
@@ -5409,7 +5400,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -5426,10 +5417,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -5443,10 +5434,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>0</v>
@@ -5477,7 +5468,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>25</v>
@@ -5494,7 +5485,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
@@ -5511,7 +5502,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
@@ -5528,7 +5519,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>29</v>
@@ -5839,10 +5830,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -5856,10 +5847,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>0</v>
@@ -6007,10 +5998,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -6024,10 +6015,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -6041,10 +6032,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -6058,10 +6049,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
@@ -6075,10 +6066,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -6092,10 +6083,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
@@ -6109,10 +6100,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>0</v>
@@ -6126,10 +6117,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
@@ -6143,10 +6134,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -6160,10 +6151,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -6226,10 +6217,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -6243,10 +6234,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -6260,10 +6251,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -6277,10 +6268,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
@@ -6294,10 +6285,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -6311,10 +6302,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>0</v>
@@ -6328,10 +6319,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>0</v>
@@ -6345,10 +6336,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
@@ -6362,10 +6353,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -6379,10 +6370,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -6690,10 +6681,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -6707,10 +6698,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>0</v>
@@ -6775,10 +6766,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -6792,10 +6783,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>0</v>
@@ -6809,16 +6800,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Updated automation scripts to reflect new column(s) (Creative Size, Placement Pixel Size)
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stash\datorama-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DatoramaAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="111">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>View Based Conversions</t>
+  </si>
+  <si>
+    <t>Placement Pixel Size</t>
+  </si>
+  <si>
+    <t>Creative_Size</t>
+  </si>
+  <si>
+    <t>Creative Size</t>
   </si>
 </sst>
 </file>
@@ -1625,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,12 +1988,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -1998,10 +2007,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -2015,16 +2024,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
@@ -2032,16 +2041,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -2049,69 +2058,86 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="1" t="b">
+      <c r="C27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>0</v>
-      </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2122,10 +2148,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,12 +2503,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -2496,10 +2522,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -2513,16 +2539,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
@@ -2530,16 +2556,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -2547,10 +2573,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>0</v>
@@ -2564,13 +2590,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -2581,35 +2607,52 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2620,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,12 +3018,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -2994,10 +3037,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -3011,16 +3054,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
@@ -3028,16 +3071,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -3045,61 +3088,61 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="1" t="b">
+      <c r="C27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>0</v>
-      </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -3113,18 +3156,35 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3135,10 +3195,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,12 +3550,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -3509,10 +3569,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -3526,16 +3586,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
@@ -3543,16 +3603,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
@@ -3560,10 +3620,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>0</v>
@@ -3577,13 +3637,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -3594,27 +3654,27 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -3628,18 +3688,35 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4134,7 +4211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Domain Delivery Data Stream Changes into the branch
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="6" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="125">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -370,6 +370,48 @@
   </si>
   <si>
     <t>Media Cost</t>
+  </si>
+  <si>
+    <t>Media Cost eCPM</t>
+  </si>
+  <si>
+    <t>Media_Cost_eCPM</t>
+  </si>
+  <si>
+    <t>Third_Party_CPM_Rate</t>
+  </si>
+  <si>
+    <t>Third Party Cost</t>
+  </si>
+  <si>
+    <t>Third_Party_Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Total_Cost</t>
+  </si>
+  <si>
+    <t>Total Cost eCPM</t>
+  </si>
+  <si>
+    <t>Total_Cost_eCPM</t>
+  </si>
+  <si>
+    <t>Client_dCPM_Rate</t>
+  </si>
+  <si>
+    <t>Client Spend</t>
+  </si>
+  <si>
+    <t>Client_Spend</t>
+  </si>
+  <si>
+    <t>Client dCPM</t>
+  </si>
+  <si>
+    <t>Client_dCPM</t>
   </si>
 </sst>
 </file>
@@ -2663,10 +2705,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3188,6 +3230,142 @@
         <v>7</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3195,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3717,6 +3895,142 @@
         <v>64</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Addec Changes to Domain Delivery Datastream for Rate cards
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2310" windowHeight="7095" tabRatio="885" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Creative_Conversion_Mapper" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="123">
   <si>
     <t>sourceColumn</t>
   </si>
@@ -372,12 +372,6 @@
     <t>Media Cost</t>
   </si>
   <si>
-    <t>Media Cost eCPM</t>
-  </si>
-  <si>
-    <t>Media_Cost_eCPM</t>
-  </si>
-  <si>
     <t>Third_Party_CPM_Rate</t>
   </si>
   <si>
@@ -393,12 +387,6 @@
     <t>Total_Cost</t>
   </si>
   <si>
-    <t>Total Cost eCPM</t>
-  </si>
-  <si>
-    <t>Total_Cost_eCPM</t>
-  </si>
-  <si>
     <t>Client_dCPM_Rate</t>
   </si>
   <si>
@@ -408,10 +396,16 @@
     <t>Client_Spend</t>
   </si>
   <si>
-    <t>Client dCPM</t>
-  </si>
-  <si>
-    <t>Client_dCPM</t>
+    <t>3rd Party Rate</t>
+  </si>
+  <si>
+    <t>Client Rate</t>
+  </si>
+  <si>
+    <t>Third_Party_Rate</t>
+  </si>
+  <si>
+    <t>Client_Rate_Test</t>
   </si>
 </sst>
 </file>
@@ -2705,10 +2699,662 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,7 +3385,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -2756,7 +3402,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -2773,7 +3419,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -2790,7 +3436,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -2807,7 +3453,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -2824,7 +3470,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -2841,7 +3487,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>30</v>
@@ -2858,7 +3504,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
@@ -2875,7 +3521,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>32</v>
@@ -2892,7 +3538,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>33</v>
@@ -2909,7 +3555,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>37</v>
@@ -2926,7 +3572,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -2943,7 +3589,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -2960,7 +3606,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
@@ -2977,7 +3623,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -2994,7 +3640,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
@@ -3011,7 +3657,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
@@ -3028,7 +3674,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
@@ -3045,7 +3691,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
@@ -3062,7 +3708,7 @@
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>99</v>
@@ -3079,7 +3725,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
@@ -3096,7 +3742,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -3113,7 +3759,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
@@ -3130,7 +3776,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>25</v>
@@ -3147,7 +3793,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>26</v>
@@ -3162,9 +3808,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>74</v>
@@ -3215,7 +3861,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>63</v>
@@ -3235,7 +3881,7 @@
         <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>0</v>
@@ -3266,7 +3912,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>115</v>
@@ -3286,7 +3932,7 @@
         <v>116</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>0</v>
@@ -3303,7 +3949,7 @@
         <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>0</v>
@@ -3312,725 +3958,6 @@
         <v>64</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C34" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added all the changes for domain delivery stream
</commit_message>
<xml_diff>
--- a/Datorama_Mapping.xlsx
+++ b/Datorama_Mapping.xlsx
@@ -2702,7 +2702,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,10 +3184,10 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3201,10 +3201,10 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>